<commit_message>
Main Assignment final commit
</commit_message>
<xml_diff>
--- a/Main_Assignment/src/resources/restdata.xlsx
+++ b/Main_Assignment/src/resources/restdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manjpr\Desktop\HU_API_TESTING_TRACK\Main_Assignment\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DF6B6F-C1EF-41DF-AB45-1B66D4F3CF8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C7F30F-A236-47F4-9560-69469BECCDE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -104,15 +104,6 @@
     <t>Happy Learning</t>
   </si>
   <si>
-    <t>dummy</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>u1ssss</t>
   </si>
   <si>
@@ -159,6 +150,12 @@
   </si>
   <si>
     <t>Going</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -525,10 +522,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>987654321</v>
@@ -537,15 +534,15 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>876543219</v>
@@ -554,15 +551,15 @@
         <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>765432198</v>
@@ -571,15 +568,15 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <v>654321987</v>
@@ -588,15 +585,15 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6">
         <v>543219876</v>
@@ -605,7 +602,7 @@
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -626,7 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D22CCFF-88F2-4360-AD81-3BA3192D4414}">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -642,7 +639,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
@@ -748,36 +745,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA23531-EFC8-4577-87E2-D97C13E2583A}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30.453125" customWidth="1"/>
     <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2">
         <v>123456789</v>
       </c>
+      <c r="D2">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{153C3A78-429B-42C5-9739-09BBC3C913F0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>